<commit_message>
cap nhat bai 1.3
</commit_message>
<xml_diff>
--- a/Chapter_1/GoshN/Chapter1/src/Code 1.4.xlsx
+++ b/Chapter_1/GoshN/Chapter1/src/Code 1.4.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncson\Desktop\Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncson\Desktop\Code\FUNiX_ReadBook_JavaIntro\Chapter_1\GoshN\Chapter1\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
   <si>
     <t>Bài 6</t>
   </si>
@@ -109,6 +109,45 @@
   </si>
   <si>
     <t>hoàn thành điều kiện nên kết thúc vòng lặp for</t>
+  </si>
+  <si>
+    <t>Bài 28</t>
+  </si>
+  <si>
+    <t>Kết quả 517</t>
+  </si>
+  <si>
+    <t>Bài 32</t>
+  </si>
+  <si>
+    <t>Bài 33</t>
+  </si>
+  <si>
+    <t>Không hiểu bài 8 nào</t>
+  </si>
+  <si>
+    <t>bài 34</t>
+  </si>
+  <si>
+    <t>Không hiểu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bài 35 </t>
+  </si>
+  <si>
+    <t>Hoang Mang</t>
+  </si>
+  <si>
+    <t>Bài 36</t>
+  </si>
+  <si>
+    <t>Chưa hiểu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bài 37 </t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -515,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D17"/>
+  <dimension ref="A2:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,6 +636,71 @@
       </c>
       <c r="B17" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -608,7 +712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>

</xml_diff>